<commit_message>
add some more data
</commit_message>
<xml_diff>
--- a/inventories.xlsx
+++ b/inventories.xlsx
@@ -693,9 +693,9 @@
   <dimension ref="A1:P57"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+      <selection pane="bottomLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -705,7 +705,7 @@
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.1938775510204"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.6887755102041"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="true" max="6" min="6" style="0" width="0"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="78.5663265306122"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.1989795918367"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.8775510204082"/>

</xml_diff>